<commit_message>
Updated SimX and Solidworks Models
</commit_message>
<xml_diff>
--- a/Mechanical/3D Model/Model 2/Mass Analysis.xlsx
+++ b/Mechanical/3D Model/Model 2/Mass Analysis.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danzn\Desktop\Final Project\ARMFLEX9000\Mechanical\3D Model\Model 2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danzn\Desktop\ARMFLEX9000\Mechanical\3D Model\Model 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33D4592B-79DE-4D66-B1F0-59BF4F01206E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{299190FE-D225-4F41-A372-3EF940A46BD1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25044" yWindow="5652" windowWidth="30960" windowHeight="12204" xr2:uid="{B3E33D88-83A3-41BC-A8DD-9DF247FD2043}"/>
+    <workbookView xWindow="10320" yWindow="4476" windowWidth="30960" windowHeight="12204" xr2:uid="{B3E33D88-83A3-41BC-A8DD-9DF247FD2043}"/>
   </bookViews>
   <sheets>
     <sheet name="Analysis" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="106">
   <si>
     <t>BaseArmMotor</t>
   </si>
@@ -125,256 +125,268 @@
     </r>
   </si>
   <si>
-    <t>Mass = 78.96 grams</t>
-  </si>
-  <si>
-    <t>Volume = 74788.99 cubic millimeters</t>
-  </si>
-  <si>
-    <t>Surface area = 41822.98  square millimeters</t>
-  </si>
-  <si>
-    <t>X = -29.23</t>
-  </si>
-  <si>
-    <t>Y = 16.54</t>
-  </si>
-  <si>
-    <t>Z = -103.64</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Ix = (-0.28, -0.22,  0.93)   </t>
-  </si>
-  <si>
-    <t>Px = 88179.38</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Iy = ( 0.95,  0.10,  0.31)   </t>
-  </si>
-  <si>
-    <t>Py = 214308.37</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Iz = (-0.16,  0.97,  0.18)   </t>
-  </si>
-  <si>
-    <t>Pz = 289859.50</t>
-  </si>
-  <si>
-    <t>Lxx = 206201.96</t>
-  </si>
-  <si>
-    <t>Lxy = 19859.83</t>
-  </si>
-  <si>
-    <t>Lxz = -30993.86</t>
-  </si>
-  <si>
-    <t>Lyx = 19859.83</t>
-  </si>
-  <si>
-    <t>Lyy = 278927.31</t>
-  </si>
-  <si>
-    <t>Lyz = -39979.73</t>
-  </si>
-  <si>
-    <t>Lzx = -30993.86</t>
-  </si>
-  <si>
-    <t>Lzy = -39979.73</t>
-  </si>
-  <si>
-    <t>Lzz = 107217.98</t>
-  </si>
-  <si>
-    <t>Ixx = 1075929.34</t>
-  </si>
-  <si>
-    <t>Ixy = -18317.37</t>
-  </si>
-  <si>
-    <t>Ixz = 208235.36</t>
-  </si>
-  <si>
-    <t>Iyx = -18317.37</t>
-  </si>
-  <si>
-    <t>Iyy = 1194534.08</t>
-  </si>
-  <si>
-    <t>Iyz = -175327.54</t>
-  </si>
-  <si>
-    <t>Izx = 208235.36</t>
-  </si>
-  <si>
-    <t>Izy = -175327.54</t>
-  </si>
-  <si>
-    <t>Izz = 196296.10</t>
-  </si>
-  <si>
-    <t>Mass = 48.23 grams</t>
-  </si>
-  <si>
-    <t>Volume = 45740.37 cubic millimeters</t>
-  </si>
-  <si>
-    <t>Surface area = 27675.43  square millimeters</t>
-  </si>
-  <si>
-    <t>X = 0.00</t>
-  </si>
-  <si>
-    <t>Y = 14.27</t>
-  </si>
-  <si>
-    <t>Z = -77.54</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Ix = ( 0.00, -0.25,  0.97)   </t>
-  </si>
-  <si>
-    <t>Px = 15192.69</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Iy = ( 1.00,  0.00,  0.00)   </t>
-  </si>
-  <si>
-    <t>Py = 78347.02</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Iz = ( 0.00,  0.97,  0.25)   </t>
-  </si>
-  <si>
-    <t>Pz = 82330.19</t>
-  </si>
-  <si>
-    <t>Lxx = 78347.02</t>
-  </si>
-  <si>
-    <t>Lxy = 0.88</t>
-  </si>
-  <si>
-    <t>Lxz = 0.00</t>
-  </si>
-  <si>
-    <t>Lyx = 0.88</t>
-  </si>
-  <si>
-    <t>Lyy = 78189.11</t>
-  </si>
-  <si>
-    <t>Lyz = -16151.56</t>
-  </si>
-  <si>
-    <t>Lzx = 0.00</t>
-  </si>
-  <si>
-    <t>Lzy = -16151.56</t>
-  </si>
-  <si>
-    <t>Lzz = 19333.76</t>
-  </si>
-  <si>
-    <t>Ixx = 378170.12</t>
-  </si>
-  <si>
-    <t>Ixy = 0.88</t>
-  </si>
-  <si>
-    <t>Ixz = 0.00</t>
-  </si>
-  <si>
-    <t>Iyx = 0.88</t>
-  </si>
-  <si>
-    <t>Iyy = 368190.38</t>
-  </si>
-  <si>
-    <t>Iyz = -69521.45</t>
-  </si>
-  <si>
-    <t>Izx = 0.00</t>
-  </si>
-  <si>
-    <t>Izy = -69521.45</t>
-  </si>
-  <si>
-    <t>Izz = 29155.60</t>
-  </si>
-  <si>
-    <t>Mass = 24.78 grams</t>
-  </si>
-  <si>
-    <t>Volume = 23491.75 cubic millimeters</t>
-  </si>
-  <si>
-    <t>Surface area = 16647.89  square millimeters</t>
-  </si>
-  <si>
-    <t>Y = 17.53</t>
-  </si>
-  <si>
-    <t>Z = -14.26</t>
-  </si>
-  <si>
-    <t>Px = 6868.15</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Iy = ( 0.01,  0.63, -0.78)   </t>
-  </si>
-  <si>
-    <t>Py = 8273.57</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Iz = ( 0.00,  0.78,  0.63)   </t>
-  </si>
-  <si>
-    <t>Pz = 10207.49</t>
-  </si>
-  <si>
-    <t>Lxx = 6868.31</t>
-  </si>
-  <si>
-    <t>Lxy = -18.60</t>
-  </si>
-  <si>
-    <t>Lyx = -18.60</t>
-  </si>
-  <si>
-    <t>Lyy = 9451.66</t>
-  </si>
-  <si>
-    <t>Lyz = -943.63</t>
-  </si>
-  <si>
-    <t>Lzy = -943.63</t>
-  </si>
-  <si>
-    <t>Lzz = 9029.24</t>
-  </si>
-  <si>
-    <t>Ixx = 19518.47</t>
-  </si>
-  <si>
-    <t>Ixy = -18.60</t>
-  </si>
-  <si>
-    <t>Iyx = -18.60</t>
-  </si>
-  <si>
-    <t>Iyy = 14489.18</t>
-  </si>
-  <si>
-    <t>Iyz = -7136.27</t>
-  </si>
-  <si>
-    <t>Izy = -7136.27</t>
-  </si>
-  <si>
-    <t>Izz = 16641.88</t>
+    <t>Mass = 89.53 grams</t>
+  </si>
+  <si>
+    <t>Volume = 84705.90 cubic millimeters</t>
+  </si>
+  <si>
+    <t>Surface area = 48550.63  square millimeters</t>
+  </si>
+  <si>
+    <t>Y = 15.20</t>
+  </si>
+  <si>
+    <t>Mass = 52.42 grams</t>
+  </si>
+  <si>
+    <t>Volume = 49683.44 cubic millimeters</t>
+  </si>
+  <si>
+    <t>Surface area = 31068.19  square millimeters</t>
+  </si>
+  <si>
+    <t>X = -0.01</t>
+  </si>
+  <si>
+    <t>Y = 12.86</t>
+  </si>
+  <si>
+    <t>Z = -75.20</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ix = ( 0.00, -0.23,  0.97)   </t>
+  </si>
+  <si>
+    <t>Lxz = -5.23</t>
+  </si>
+  <si>
+    <t>Lyz = -18496.44</t>
+  </si>
+  <si>
+    <t>Lzx = -5.23</t>
+  </si>
+  <si>
+    <t>Lzy = -18496.44</t>
+  </si>
+  <si>
+    <t>Ixz = 31.81</t>
+  </si>
+  <si>
+    <t>Iyz = -69190.53</t>
+  </si>
+  <si>
+    <t>Izx = 31.81</t>
+  </si>
+  <si>
+    <t>Izy = -69190.53</t>
+  </si>
+  <si>
+    <t>Mass = 23.88 grams</t>
+  </si>
+  <si>
+    <t>Volume = 22660.99 cubic millimeters</t>
+  </si>
+  <si>
+    <t>Surface area = 17185.76  square millimeters</t>
+  </si>
+  <si>
+    <t>Y = 17.44</t>
+  </si>
+  <si>
+    <t>Z = -16.94</t>
+  </si>
+  <si>
+    <t>Px = 7302.66</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Iy = ( 0.01,  0.61, -0.79)   </t>
+  </si>
+  <si>
+    <t>Py = 8459.94</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Iz = ( 0.01,  0.79,  0.61)   </t>
+  </si>
+  <si>
+    <t>Pz = 10744.91</t>
+  </si>
+  <si>
+    <t>Lxx = 7302.85</t>
+  </si>
+  <si>
+    <t>Lxy = -20.33</t>
+  </si>
+  <si>
+    <t>Lxz = -2.07</t>
+  </si>
+  <si>
+    <t>Lyx = -20.33</t>
+  </si>
+  <si>
+    <t>Lyy = 9896.73</t>
+  </si>
+  <si>
+    <t>Lyz = -1103.91</t>
+  </si>
+  <si>
+    <t>Lzx = -2.07</t>
+  </si>
+  <si>
+    <t>Lzy = -1103.91</t>
+  </si>
+  <si>
+    <t>Lzz = 9307.92</t>
+  </si>
+  <si>
+    <t>Ixx = 21422.46</t>
+  </si>
+  <si>
+    <t>Ixy = -23.63</t>
+  </si>
+  <si>
+    <t>Ixz = 1.14</t>
+  </si>
+  <si>
+    <t>Iyx = -23.63</t>
+  </si>
+  <si>
+    <t>Iyy = 16750.34</t>
+  </si>
+  <si>
+    <t>Iyz = -8160.70</t>
+  </si>
+  <si>
+    <t>Izx = 1.14</t>
+  </si>
+  <si>
+    <t>Izy = -8160.70</t>
+  </si>
+  <si>
+    <t>Izz = 16573.93</t>
+  </si>
+  <si>
+    <t>X = -26.85</t>
+  </si>
+  <si>
+    <t>Z = -113.59</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ix = (-0.18, -0.18,  0.97)   </t>
+  </si>
+  <si>
+    <t>Px = 83808.65</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Iy = ( 0.97,  0.13,  0.20)   </t>
+  </si>
+  <si>
+    <t>Py = 326016.31</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Iz = (-0.16,  0.98,  0.15)   </t>
+  </si>
+  <si>
+    <t>Pz = 395954.44</t>
+  </si>
+  <si>
+    <t>Lxx = 320180.99</t>
+  </si>
+  <si>
+    <t>Lxy = 18533.50</t>
+  </si>
+  <si>
+    <t>Lxz = -39900.58</t>
+  </si>
+  <si>
+    <t>Lyx = 18533.50</t>
+  </si>
+  <si>
+    <t>Lyy = 384932.49</t>
+  </si>
+  <si>
+    <t>Lyz = -51946.31</t>
+  </si>
+  <si>
+    <t>Lzx = -39900.58</t>
+  </si>
+  <si>
+    <t>Lzy = -51946.31</t>
+  </si>
+  <si>
+    <t>Lzz = 100665.93</t>
+  </si>
+  <si>
+    <t>Ixx = 1496094.97</t>
+  </si>
+  <si>
+    <t>Ixy = -17996.70</t>
+  </si>
+  <si>
+    <t>Ixz = 233171.33</t>
+  </si>
+  <si>
+    <t>Iyx = -17996.70</t>
+  </si>
+  <si>
+    <t>Iyy = 1604720.43</t>
+  </si>
+  <si>
+    <t>Iyz = -206488.57</t>
+  </si>
+  <si>
+    <t>Izx = 233171.33</t>
+  </si>
+  <si>
+    <t>Izy = -206488.57</t>
+  </si>
+  <si>
+    <t>Izz = 185887.67</t>
+  </si>
+  <si>
+    <t>Px = 11790.92</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Iy = ( 0.04, -0.97, -0.23)   </t>
+  </si>
+  <si>
+    <t>Py = 94991.62</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Iz = ( 1.00,  0.04,  0.01)   </t>
+  </si>
+  <si>
+    <t>Pz = 95348.49</t>
+  </si>
+  <si>
+    <t>Lxx = 95347.94</t>
+  </si>
+  <si>
+    <t>Lxy = -13.10</t>
+  </si>
+  <si>
+    <t>Lyx = -13.10</t>
+  </si>
+  <si>
+    <t>Lyy = 90654.04</t>
+  </si>
+  <si>
+    <t>Lzz = 16129.04</t>
+  </si>
+  <si>
+    <t>Ixx = 400510.75</t>
+  </si>
+  <si>
+    <t>Ixy = -19.43</t>
+  </si>
+  <si>
+    <t>Iyx = -19.43</t>
+  </si>
+  <si>
+    <t>Iyy = 387149.29</t>
+  </si>
+  <si>
+    <t>Izz = 24796.61</t>
   </si>
 </sst>
 </file>
@@ -742,7 +754,7 @@
   <dimension ref="B2:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -770,7 +782,7 @@
       </c>
       <c r="C3" t="str">
         <f>BaseArmMotor!D32</f>
-        <v>Iyy = 1194534.08</v>
+        <v>Iyy = 1604720.43</v>
       </c>
       <c r="D3">
         <v>0.08</v>
@@ -784,8 +796,8 @@
         <v>1</v>
       </c>
       <c r="C4" t="str">
-        <f>ForeArmMotor!D32</f>
-        <v>Iyy = 368190.38</v>
+        <f>ForeArmMotor!E33</f>
+        <v>Izz = 24796.61</v>
       </c>
       <c r="D4">
         <v>0.08</v>
@@ -799,8 +811,8 @@
         <v>2</v>
       </c>
       <c r="C5" t="str">
-        <f>GripperMotor!D32</f>
-        <v>Iyy = 14489.18</v>
+        <f>GripperMotor!C31</f>
+        <v>Ixx = 21422.46</v>
       </c>
       <c r="D5">
         <v>0.08</v>
@@ -825,7 +837,7 @@
   <dimension ref="B2:E33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H36" sqref="H36"/>
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -867,17 +879,17 @@
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
-        <v>21</v>
+        <v>65</v>
       </c>
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
-        <v>23</v>
+        <v>66</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
@@ -892,26 +904,26 @@
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
-        <v>24</v>
+        <v>67</v>
       </c>
       <c r="D19" t="s">
-        <v>25</v>
+        <v>68</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
-        <v>26</v>
+        <v>69</v>
       </c>
       <c r="D20" t="s">
-        <v>27</v>
+        <v>70</v>
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
-        <v>28</v>
+        <v>71</v>
       </c>
       <c r="D21" t="s">
-        <v>29</v>
+        <v>72</v>
       </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
@@ -926,35 +938,35 @@
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
-        <v>30</v>
+        <v>73</v>
       </c>
       <c r="D25" t="s">
-        <v>31</v>
+        <v>74</v>
       </c>
       <c r="E25" t="s">
-        <v>32</v>
+        <v>75</v>
       </c>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C26" t="s">
-        <v>33</v>
+        <v>76</v>
       </c>
       <c r="D26" t="s">
-        <v>34</v>
+        <v>77</v>
       </c>
       <c r="E26" t="s">
-        <v>35</v>
+        <v>78</v>
       </c>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
-        <v>36</v>
+        <v>79</v>
       </c>
       <c r="D27" t="s">
-        <v>37</v>
+        <v>80</v>
       </c>
       <c r="E27" t="s">
-        <v>38</v>
+        <v>81</v>
       </c>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.25">
@@ -969,35 +981,35 @@
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C31" t="s">
-        <v>39</v>
+        <v>82</v>
       </c>
       <c r="D31" t="s">
-        <v>40</v>
+        <v>83</v>
       </c>
       <c r="E31" t="s">
-        <v>41</v>
+        <v>84</v>
       </c>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C32" t="s">
-        <v>42</v>
+        <v>85</v>
       </c>
       <c r="D32" t="s">
-        <v>43</v>
+        <v>86</v>
       </c>
       <c r="E32" t="s">
-        <v>44</v>
+        <v>87</v>
       </c>
     </row>
     <row r="33" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C33" t="s">
-        <v>45</v>
+        <v>88</v>
       </c>
       <c r="D33" t="s">
-        <v>46</v>
+        <v>89</v>
       </c>
       <c r="E33" t="s">
-        <v>47</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -1010,7 +1022,7 @@
   <dimension ref="B2:E33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I31" sqref="I31"/>
+      <selection activeCell="B2" sqref="B2:E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1032,17 +1044,17 @@
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>48</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>49</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>50</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.25">
@@ -1052,17 +1064,17 @@
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
-        <v>51</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
-        <v>52</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
-        <v>53</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
@@ -1077,26 +1089,26 @@
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
-        <v>54</v>
+        <v>28</v>
       </c>
       <c r="D19" t="s">
-        <v>55</v>
+        <v>91</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
-        <v>56</v>
+        <v>92</v>
       </c>
       <c r="D20" t="s">
-        <v>57</v>
+        <v>93</v>
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
-        <v>58</v>
+        <v>94</v>
       </c>
       <c r="D21" t="s">
-        <v>59</v>
+        <v>95</v>
       </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
@@ -1111,35 +1123,35 @@
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
-        <v>60</v>
+        <v>96</v>
       </c>
       <c r="D25" t="s">
-        <v>61</v>
+        <v>97</v>
       </c>
       <c r="E25" t="s">
-        <v>62</v>
+        <v>29</v>
       </c>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C26" t="s">
-        <v>63</v>
+        <v>98</v>
       </c>
       <c r="D26" t="s">
-        <v>64</v>
+        <v>99</v>
       </c>
       <c r="E26" t="s">
-        <v>65</v>
+        <v>30</v>
       </c>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
-        <v>66</v>
+        <v>31</v>
       </c>
       <c r="D27" t="s">
-        <v>67</v>
+        <v>32</v>
       </c>
       <c r="E27" t="s">
-        <v>68</v>
+        <v>100</v>
       </c>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.25">
@@ -1154,35 +1166,35 @@
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C31" t="s">
-        <v>69</v>
+        <v>101</v>
       </c>
       <c r="D31" t="s">
-        <v>70</v>
+        <v>102</v>
       </c>
       <c r="E31" t="s">
-        <v>71</v>
+        <v>33</v>
       </c>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C32" t="s">
-        <v>72</v>
+        <v>103</v>
       </c>
       <c r="D32" t="s">
-        <v>73</v>
+        <v>104</v>
       </c>
       <c r="E32" t="s">
-        <v>74</v>
+        <v>34</v>
       </c>
     </row>
     <row r="33" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C33" t="s">
-        <v>75</v>
+        <v>35</v>
       </c>
       <c r="D33" t="s">
-        <v>76</v>
+        <v>36</v>
       </c>
       <c r="E33" t="s">
-        <v>77</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -1195,7 +1207,7 @@
   <dimension ref="B2:E33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H33" sqref="H33"/>
+      <selection activeCell="G40" sqref="G40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1217,17 +1229,17 @@
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>78</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>79</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>80</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.25">
@@ -1237,17 +1249,17 @@
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
-        <v>51</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
-        <v>81</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
-        <v>82</v>
+        <v>41</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
@@ -1265,23 +1277,23 @@
         <v>14</v>
       </c>
       <c r="D19" t="s">
-        <v>83</v>
+        <v>42</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
-        <v>84</v>
+        <v>43</v>
       </c>
       <c r="D20" t="s">
-        <v>85</v>
+        <v>44</v>
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
-        <v>86</v>
+        <v>45</v>
       </c>
       <c r="D21" t="s">
-        <v>87</v>
+        <v>46</v>
       </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
@@ -1296,35 +1308,35 @@
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
-        <v>88</v>
+        <v>47</v>
       </c>
       <c r="D25" t="s">
-        <v>89</v>
+        <v>48</v>
       </c>
       <c r="E25" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C26" t="s">
-        <v>90</v>
+        <v>50</v>
       </c>
       <c r="D26" t="s">
-        <v>91</v>
+        <v>51</v>
       </c>
       <c r="E26" t="s">
-        <v>92</v>
+        <v>52</v>
       </c>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="D27" t="s">
-        <v>93</v>
+        <v>54</v>
       </c>
       <c r="E27" t="s">
-        <v>94</v>
+        <v>55</v>
       </c>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.25">
@@ -1339,35 +1351,35 @@
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C31" t="s">
-        <v>95</v>
+        <v>56</v>
       </c>
       <c r="D31" t="s">
-        <v>96</v>
+        <v>57</v>
       </c>
       <c r="E31" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C32" t="s">
-        <v>97</v>
+        <v>59</v>
       </c>
       <c r="D32" t="s">
-        <v>98</v>
+        <v>60</v>
       </c>
       <c r="E32" t="s">
-        <v>99</v>
+        <v>61</v>
       </c>
     </row>
     <row r="33" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C33" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="D33" t="s">
-        <v>100</v>
+        <v>63</v>
       </c>
       <c r="E33" t="s">
-        <v>101</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>